<commit_message>
reconfigured report to use a single fiscal year
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_21_rpt_PA_Billing-Historical.xlsx
+++ b/backend/reports/xlsx/Tab_21_rpt_PA_Billing-Historical.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleshapka/Development/github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F418D4AC-72EE-8B48-9976-5354A6CDD679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78177E02-7A73-1A4E-B6E2-030C6EF8AD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76100" yWindow="1400" windowWidth="34560" windowHeight="19780" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="76720" yWindow="620" windowWidth="34560" windowHeight="19780" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>{#fy2=d.report[i=-1].budget_fiscal}</t>
+  </si>
+  <si>
+    <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>{$t.q1_total}</t>
+  </si>
+  <si>
+    <t>{$t.q2_total}</t>
+  </si>
+  <si>
+    <t>{$t.q3_total}</t>
+  </si>
+  <si>
+    <t>{$t.q4_total}</t>
+  </si>
+  <si>
+    <t>{$t.grand_total}</t>
+  </si>
+  <si>
+    <t>{#t=d.report_totals[i]}</t>
   </si>
 </sst>
 </file>
@@ -114,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +164,11 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -241,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -277,6 +303,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +687,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -748,6 +777,28 @@
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
     </row>
+    <row r="5" spans="1:8" ht="17" thickBot="1">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>0</v>
@@ -759,7 +810,9 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">

</xml_diff>